<commit_message>
Vue UI Testing V2
</commit_message>
<xml_diff>
--- a/documents/react-unit-testing-sheet.xlsx
+++ b/documents/react-unit-testing-sheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Downloads\Github Projects\SIS-Frontend\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A79A904-C781-4F02-9231-72CD1E40B7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7F036-928E-43AA-8F80-2FA7420FAE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
   </bookViews>
   <sheets>
     <sheet name="UI Test Case" sheetId="1" r:id="rId1"/>
     <sheet name="UI Test Case Photo" sheetId="2" r:id="rId2"/>
     <sheet name="Vue UI Test Cases" sheetId="4" r:id="rId3"/>
+    <sheet name="Vue UI Test Case Photo" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1307,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE04282-0A33-4622-BE62-517B943F70CB}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -1602,4 +1603,18 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657941E-CD4E-4457-A34F-89D4E3469D88}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Vue UI Testing V3
</commit_message>
<xml_diff>
--- a/documents/react-unit-testing-sheet.xlsx
+++ b/documents/react-unit-testing-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Downloads\Github Projects\SIS-Frontend\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7F036-928E-43AA-8F80-2FA7420FAE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0493BB4-AF5D-4A48-9997-C125007DC58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="3" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
   </bookViews>
   <sheets>
     <sheet name="UI Test Case" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -1308,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE04282-0A33-4622-BE62-517B943F70CB}">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1367,12 +1367,8 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -1388,12 +1384,8 @@
       <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1409,12 +1401,8 @@
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
@@ -1430,12 +1418,8 @@
       <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1451,15 +1435,11 @@
       <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -1472,12 +1452,8 @@
       <c r="D8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1493,12 +1469,8 @@
       <c r="D9" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1534,12 +1506,8 @@
       <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1609,7 +1577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657941E-CD4E-4457-A34F-89D4E3469D88}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Vue UI Testing V4
</commit_message>
<xml_diff>
--- a/documents/react-unit-testing-sheet.xlsx
+++ b/documents/react-unit-testing-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Downloads\Github Projects\SIS-Frontend\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0493BB4-AF5D-4A48-9997-C125007DC58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7603F01-B523-4EB4-8CD0-626A0FB92F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
   <si>
     <t>Description</t>
   </si>
@@ -203,6 +203,66 @@
   </si>
   <si>
     <t>Please scroll down for Test Cases Photos</t>
+  </si>
+  <si>
+    <t>Yes website does appear when entered into the URL</t>
+  </si>
+  <si>
+    <t>Yes the calenar button is working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes the profile button is working and direct you to a calendar </t>
+  </si>
+  <si>
+    <t>Th profile page allow you to ammend and change profile details</t>
+  </si>
+  <si>
+    <t>The task button work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The calendars drag and drop feature works properly </t>
+  </si>
+  <si>
+    <t>The calendar lets me look at a daily, weekly and monthly view</t>
+  </si>
+  <si>
+    <t>Account creation page</t>
+  </si>
+  <si>
+    <t>Testing that you can sign up</t>
+  </si>
+  <si>
+    <t>That when I enter all in the details to create an account and click sign up it should work</t>
+  </si>
+  <si>
+    <t>The sign up process worked but it required a capital letter in the password</t>
+  </si>
+  <si>
+    <t>We can select and unselect the different type of events</t>
+  </si>
+  <si>
+    <t>Select and unselect  event types</t>
+  </si>
+  <si>
+    <t>We should be able to select and unselect event types</t>
+  </si>
+  <si>
+    <t>Yes we were able to select and unselect event types</t>
+  </si>
+  <si>
+    <t>FD009</t>
+  </si>
+  <si>
+    <t>Selecting invidiual days on the calendar app</t>
+  </si>
+  <si>
+    <t>We can select individual days within our calendar app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The individuals days on the calendar can be selected and </t>
+  </si>
+  <si>
+    <t>Yes the individual days on the calanedar can be selected</t>
   </si>
 </sst>
 </file>
@@ -635,6 +695,363 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>88901</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>410891</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71DF9B37-AB50-77F5-EDB7-D7E1E5128D36}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="438150" y="641351"/>
+          <a:ext cx="5459141" cy="4184650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>146654</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>43353</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA8E8E55-68E0-8BBD-05D8-D3818CD49920}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6445250" y="863600"/>
+          <a:ext cx="8331804" cy="3783503"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1452B5B-590E-F70B-5CCF-317B17DD67B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="603250" y="5689600"/>
+          <a:ext cx="7054850" cy="3721100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>222731</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>72033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38734155-2EDB-9796-D496-404309F12F44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8578850" y="5695951"/>
+          <a:ext cx="6883881" cy="3215282"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>596901</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>44451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>241301</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>50801</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A81DEE4E-C15A-4842-E802-BCA6DDCB56D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="596901" y="10541001"/>
+          <a:ext cx="6350000" cy="2768600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>142970</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B437B5F6-7486-9DE1-0748-04D794A2599A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7956550" y="10439401"/>
+          <a:ext cx="6381750" cy="3883119"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>109061</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{038D3384-6356-0BFD-4A7E-0DD2031BC1E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="15652750"/>
+          <a:ext cx="6205061" cy="2457450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>419101</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>21575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF7D685-EF76-65FA-F08A-75A0B6B7280D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315201" y="15652750"/>
+          <a:ext cx="1638300" cy="4441175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1236,7 +1653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A41BFC6-51CE-46E6-87ED-11C918896455}">
   <dimension ref="B2:W84"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -1306,10 +1723,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE04282-0A33-4622-BE62-517B943F70CB}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1367,8 +1784,12 @@
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="58" x14ac:dyDescent="0.35">
@@ -1376,138 +1797,188 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="E7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="E9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+    <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1519,22 +1990,36 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row r="14" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="3"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1564,10 +2049,37 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1575,14 +2087,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657941E-CD4E-4457-A34F-89D4E3469D88}">
-  <dimension ref="A1"/>
+  <dimension ref="A3:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="Q99" sqref="Q99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="L3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="O30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B56" t="s">
+        <v>44</v>
+      </c>
+      <c r="N56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="B84" t="s">
+        <v>38</v>
+      </c>
+      <c r="M84" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Vue UI Testing V5
</commit_message>
<xml_diff>
--- a/documents/react-unit-testing-sheet.xlsx
+++ b/documents/react-unit-testing-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Downloads\Github Projects\SIS-Frontend\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7603F01-B523-4EB4-8CD0-626A0FB92F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AFBCB7-D268-4CA5-BF46-554AFCAA9C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" activeTab="2" xr2:uid="{04AE5837-ECD8-4336-A4A9-F56AB5496548}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
   <si>
     <t>Description</t>
   </si>
@@ -263,6 +263,30 @@
   </si>
   <si>
     <t>Yes the individual days on the calanedar can be selected</t>
+  </si>
+  <si>
+    <t>You can create calendar events</t>
+  </si>
+  <si>
+    <t>Yo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You can create calendar events </t>
+  </si>
+  <si>
+    <t>The calendar event can be created and the event can be amended</t>
+  </si>
+  <si>
+    <t>Yes a calendar event can be made and details can be added</t>
+  </si>
+  <si>
+    <t>FD010</t>
+  </si>
+  <si>
+    <t>FD011</t>
+  </si>
+  <si>
+    <t>FD0010</t>
   </si>
 </sst>
 </file>
@@ -787,50 +811,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>603250</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1452B5B-590E-F70B-5CCF-317B17DD67B3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="603250" y="5689600"/>
-          <a:ext cx="7054850" cy="3721100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>44450</xdr:colOff>
       <xdr:row>30</xdr:row>
@@ -856,7 +836,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -900,7 +880,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -944,7 +924,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -963,16 +943,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>109061</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>90011</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -988,14 +968,14 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="15652750"/>
+          <a:off x="5467350" y="15875000"/>
           <a:ext cx="6205061" cy="2457450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1007,16 +987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>374651</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>419101</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>21575</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>184151</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>66025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1032,6 +1012,50 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11957051" y="16065500"/>
+          <a:ext cx="1638300" cy="4441175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>500707</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>178137</xdr:colOff>
+      <xdr:row>133</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1982422B-1226-7FED-BA3D-58CA860187A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
@@ -1039,8 +1063,140 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7315201" y="15652750"/>
-          <a:ext cx="1638300" cy="4441175"/>
+          <a:off x="500707" y="19773900"/>
+          <a:ext cx="4554230" cy="4730750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533153</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3239C8-6C75-F6AD-3840-96EFB4B37C27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="5892800"/>
+          <a:ext cx="5409953" cy="3289300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>418213</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F80FBEDA-CF33-2525-63FA-13932FA83257}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="558800" y="15779750"/>
+          <a:ext cx="4126613" cy="2825750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>330342</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87567CBC-A34C-023D-26EE-166BA227C0A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="19748500"/>
+          <a:ext cx="2768742" cy="1981302"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1723,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE04282-0A33-4622-BE62-517B943F70CB}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1753,7 +1909,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -1815,7 +1971,7 @@
     </row>
     <row r="5" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
@@ -1836,7 +1992,7 @@
     </row>
     <row r="6" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -1857,7 +2013,7 @@
     </row>
     <row r="7" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>24</v>
@@ -1878,7 +2034,7 @@
     </row>
     <row r="8" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
@@ -1899,7 +2055,7 @@
     </row>
     <row r="9" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>34</v>
@@ -1920,7 +2076,7 @@
     </row>
     <row r="10" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>39</v>
@@ -1941,7 +2097,7 @@
     </row>
     <row r="11" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>67</v>
@@ -1962,7 +2118,7 @@
     </row>
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>71</v>
@@ -1981,63 +2137,75 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+    <row r="13" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="3"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
+    <row r="16" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="3"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+    <row r="17" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2076,21 +2244,40 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A16:B16"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6657941E-CD4E-4457-A34F-89D4E3469D88}">
-  <dimension ref="A3:P84"/>
+  <dimension ref="A3:U136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q99" sqref="Q99"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="P107" sqref="P107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,12 +2330,30 @@
         <v>45</v>
       </c>
     </row>
-    <row r="84" spans="2:13" x14ac:dyDescent="0.35">
-      <c r="B84" t="s">
+    <row r="85" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B85" t="s">
         <v>38</v>
       </c>
-      <c r="M84" t="s">
+      <c r="J85" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="U86" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="106" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B106" t="s">
+        <v>82</v>
+      </c>
+      <c r="K106" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B136" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>